<commit_message>
Life Point Prefab Pickup Added
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Loot_All.xlsb.xlsx
+++ b/Assets/Resources/CSV/Loot_All.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imane\Documents\GitHub\2022-2023-A5-Procedural-Team3\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B053E9F8-8E48-4A7B-88BA-67F9903BD666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7C3EA8-A68C-44FA-87B0-EF91BA061BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="1500" windowWidth="13680" windowHeight="11385" activeTab="2" xr2:uid="{5CA59659-9F81-4D77-B917-712C15DA2AAF}"/>
+    <workbookView xWindow="75" yWindow="1500" windowWidth="14700" windowHeight="11385" activeTab="2" xr2:uid="{5CA59659-9F81-4D77-B917-712C15DA2AAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities_Dungeon_1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -151,9 +151,6 @@
     <t>RARITY</t>
   </si>
   <si>
-    <t>Assets/Scripts/LootTable/Loot/L_Heart_1.asset</t>
-  </si>
-  <si>
     <t>COMMON</t>
   </si>
   <si>
@@ -173,6 +170,18 @@
   </si>
   <si>
     <t>RARE</t>
+  </si>
+  <si>
+    <t>Assets/Prefabs/Pickups/LifePoint.prefab</t>
+  </si>
+  <si>
+    <t>Assets/Prefabs/Pickups/Key.prefab</t>
+  </si>
+  <si>
+    <t>LIFE_POINT_1</t>
+  </si>
+  <si>
+    <t>Minor Heal</t>
   </si>
 </sst>
 </file>
@@ -791,10 +800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED11733-B24E-4C72-B58D-C813EF0670E1}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" activeCellId="1" sqref="D8 D10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>26</v>
@@ -824,13 +833,13 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -838,13 +847,13 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -852,13 +861,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -866,13 +875,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,13 +889,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -894,27 +903,41 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Weapon Entities Added
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Loot_All.xlsb.xlsx
+++ b/Assets/Resources/CSV/Loot_All.xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imane\Documents\GitHub\2022-2023-A5-Procedural-Team3\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7C3EA8-A68C-44FA-87B0-EF91BA061BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AA87CD-3959-489D-9431-527CA4CA41C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="75" yWindow="1500" windowWidth="14700" windowHeight="11385" activeTab="2" xr2:uid="{5CA59659-9F81-4D77-B917-712C15DA2AAF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -182,6 +182,33 @@
   </si>
   <si>
     <t>Minor Heal</t>
+  </si>
+  <si>
+    <t>PISTOL_1</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>Assets/Scripts/Weapons/Pistol.prefab</t>
+  </si>
+  <si>
+    <t>MACHINE_GUN_1</t>
+  </si>
+  <si>
+    <t>SHOT_GUN_1</t>
+  </si>
+  <si>
+    <t>Assets/Scripts/Weapons/MachineGun.prefab</t>
+  </si>
+  <si>
+    <t>Assets/Scripts/Weapons/ShotGun.prefab</t>
+  </si>
+  <si>
+    <t>Machine Gun</t>
+  </si>
+  <si>
+    <t>Shot Gun</t>
   </si>
 </sst>
 </file>
@@ -800,10 +827,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED11733-B24E-4C72-B58D-C813EF0670E1}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,6 +967,48 @@
         <v>37</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bonus Drop Loot System Added
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Loot_All.xlsb.xlsx
+++ b/Assets/Resources/CSV/Loot_All.xlsb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imane\Documents\GitHub\2022-2023-A5-Procedural-Team3\Assets\Resources\CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\2022-2023-A5-Procedural-Team3\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AA87CD-3959-489D-9431-527CA4CA41C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34741763-A07B-4779-87A7-ADF8A629CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="1500" windowWidth="14700" windowHeight="11385" activeTab="2" xr2:uid="{5CA59659-9F81-4D77-B917-712C15DA2AAF}"/>
+    <workbookView xWindow="7470" yWindow="4510" windowWidth="13800" windowHeight="12110" activeTab="2" xr2:uid="{5CA59659-9F81-4D77-B917-712C15DA2AAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities_Dungeon_1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Shot Gun</t>
+  </si>
+  <si>
+    <t>BONUS_ARMOR_1</t>
   </si>
 </sst>
 </file>
@@ -607,16 +610,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="4" max="4" width="41.54296875" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -650,7 +653,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -667,7 +670,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -684,7 +687,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -715,14 +718,14 @@
       <selection activeCell="A2" sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="1" max="2" width="23.26953125" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,7 +739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -750,7 +753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -764,7 +767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -778,7 +781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -792,7 +795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -806,7 +809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -827,21 +830,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED11733-B24E-4C72-B58D-C813EF0670E1}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="48.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +858,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -869,7 +872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -883,7 +886,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -897,7 +900,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -911,7 +914,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -925,7 +928,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -939,7 +942,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -953,7 +956,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -967,7 +970,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -981,7 +984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -995,7 +998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1006,6 +1009,34 @@
         <v>56</v>
       </c>
       <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>